<commit_message>
Code for If Else Conditions
Code for If Else Conditions
</commit_message>
<xml_diff>
--- a/Project Batch daily Sheet React B10 G2.xlsx
+++ b/Project Batch daily Sheet React B10 G2.xlsx
@@ -553,7 +553,7 @@
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -573,16 +573,32 @@
         <v>45292</v>
       </c>
       <c r="D1" s="4">
-        <v>45290</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+        <v>45293</v>
+      </c>
+      <c r="E1" s="4">
+        <v>45294</v>
+      </c>
+      <c r="F1" s="4">
+        <v>45295</v>
+      </c>
+      <c r="G1" s="4">
+        <v>45296</v>
+      </c>
+      <c r="H1" s="4">
+        <v>45297</v>
+      </c>
+      <c r="I1" s="4">
+        <v>45298</v>
+      </c>
+      <c r="J1" s="4">
+        <v>45299</v>
+      </c>
+      <c r="K1" s="4">
+        <v>45300</v>
+      </c>
+      <c r="L1" s="4">
+        <v>45301</v>
+      </c>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -814,6 +830,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added code if else and switch case
Added code if else and switch case and attendance tracker
</commit_message>
<xml_diff>
--- a/Project Batch daily Sheet React B10 G2.xlsx
+++ b/Project Batch daily Sheet React B10 G2.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
   <si>
     <t>Student Name</t>
   </si>
@@ -553,7 +553,7 @@
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -621,7 +621,9 @@
       <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -651,7 +653,9 @@
       <c r="D3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -681,7 +685,9 @@
       <c r="D4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -711,7 +717,9 @@
       <c r="D5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -741,7 +749,9 @@
       <c r="D6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -771,7 +781,9 @@
       <c r="D7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -801,7 +813,9 @@
       <c r="D8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>

</xml_diff>

<commit_message>
js Objects and assignment and daily attendance
js Objects and assignment and daily attendance
</commit_message>
<xml_diff>
--- a/Project Batch daily Sheet React B10 G2.xlsx
+++ b/Project Batch daily Sheet React B10 G2.xlsx
@@ -245,12 +245,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="K8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>pooja patil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+power out</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="14">
   <si>
     <t>Student Name</t>
   </si>
@@ -289,6 +313,9 @@
   </si>
   <si>
     <t>Reshma Bhuse</t>
+  </si>
+  <si>
+    <t>1101-2024</t>
   </si>
 </sst>
 </file>
@@ -697,7 +724,7 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -737,7 +764,9 @@
       <c r="J1" s="4">
         <v>45301</v>
       </c>
-      <c r="K1" s="5"/>
+      <c r="K1" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -777,7 +806,9 @@
       <c r="J2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="7"/>
+      <c r="K2" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
@@ -817,7 +848,9 @@
       <c r="J3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="7"/>
+      <c r="K3" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
@@ -857,7 +890,9 @@
       <c r="J4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="7"/>
+      <c r="K4" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
@@ -897,7 +932,9 @@
       <c r="J5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="7"/>
+      <c r="K5" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
@@ -937,7 +974,9 @@
       <c r="J6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="7"/>
+      <c r="K6" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
@@ -977,7 +1016,9 @@
       <c r="J7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="7"/>
+      <c r="K7" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
@@ -1017,7 +1058,9 @@
       <c r="J8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="7"/>
+      <c r="K8" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>

</xml_diff>

<commit_message>
Function Constructor And assignment
Function Constructor And assignment
</commit_message>
<xml_diff>
--- a/Project Batch daily Sheet React B10 G2.xlsx
+++ b/Project Batch daily Sheet React B10 G2.xlsx
@@ -269,12 +269,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="L8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>pooja patil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+power out</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>pooja patil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+power out</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="13">
   <si>
     <t>Student Name</t>
   </si>
@@ -313,9 +361,6 @@
   </si>
   <si>
     <t>Reshma Bhuse</t>
-  </si>
-  <si>
-    <t>1101-2024</t>
   </si>
 </sst>
 </file>
@@ -724,7 +769,7 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -764,11 +809,15 @@
       <c r="J1" s="4">
         <v>45301</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="K1" s="4">
+        <v>45302</v>
+      </c>
+      <c r="L1" s="4">
+        <v>45303</v>
+      </c>
+      <c r="M1" s="4">
+        <v>45304</v>
+      </c>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
@@ -809,8 +858,12 @@
       <c r="K2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
+      <c r="L2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
@@ -851,8 +904,12 @@
       <c r="K3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
+      <c r="L3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
@@ -893,8 +950,12 @@
       <c r="K4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
+      <c r="L4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
@@ -935,8 +996,12 @@
       <c r="K5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
+      <c r="L5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
@@ -977,8 +1042,12 @@
       <c r="K6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="L6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
@@ -1019,8 +1088,12 @@
       <c r="K7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
+      <c r="L7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
@@ -1061,8 +1134,12 @@
       <c r="K8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+      <c r="L8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>

</xml_diff>

<commit_message>
for each method with arrow and callback function
for each method with arrow and callback function
</commit_message>
<xml_diff>
--- a/Project Batch daily Sheet React B10 G2.xlsx
+++ b/Project Batch daily Sheet React B10 G2.xlsx
@@ -418,7 +418,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="13">
   <si>
     <t>Student Name</t>
   </si>
@@ -533,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -543,7 +543,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -864,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -926,385 +925,401 @@
       <c r="Q1" s="4">
         <v>45308</v>
       </c>
-      <c r="R1" s="5"/>
+      <c r="R1" s="4">
+        <v>45309</v>
+      </c>
     </row>
     <row r="2" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="7" t="s">
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="R2" s="7"/>
+      <c r="J2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="R3" s="7"/>
+      <c r="C3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="7" t="s">
+      <c r="C4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="R4" s="7"/>
+      <c r="J4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="R5" s="7"/>
+      <c r="C5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="R6" s="7"/>
+      <c r="C6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="7" t="s">
+      <c r="D7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="R7" s="7"/>
+      <c r="G7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="7" t="s">
+      <c r="C8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8" s="7" t="s">
+      <c r="G8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="R8" s="7"/>
+      <c r="K8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
@@ -1313,7 +1328,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:Q8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:R8">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>